<commit_message>
added input text files for task 1
</commit_message>
<xml_diff>
--- a/Project - Nariana Sands/feature requests.xlsx
+++ b/Project - Nariana Sands/feature requests.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ysands\Desktop\Software Requirements\Task 3- Nariana Sands\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ysands\Desktop\Software Requirements\CSE7316\Project - Nariana Sands\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="frtrsf" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="162">
   <si>
     <t>Request ID</t>
   </si>
@@ -884,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,12 +3096,210 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3">
+        <f>B2+1</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B11" si="0">B3+1</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3322,7 +3520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
stopping point. This version isn't working with text files as input.
</commit_message>
<xml_diff>
--- a/Project - Nariana Sands/feature requests.xlsx
+++ b/Project - Nariana Sands/feature requests.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="frtrsf" sheetId="1" r:id="rId1"/>
     <sheet name="frtrss" sheetId="8" r:id="rId2"/>
-    <sheet name="frtess" sheetId="6" r:id="rId3"/>
-    <sheet name="frtesf" sheetId="5" r:id="rId4"/>
+    <sheet name="frtesf" sheetId="5" r:id="rId3"/>
+    <sheet name="frtess" sheetId="6" r:id="rId4"/>
     <sheet name="lrtess" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -885,7 +885,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3098,218 +3098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3">
-        <f>B2+1</f>
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B11" si="0">B3+1</f>
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A1:K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3513,6 +3303,216 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3">
+        <f>B2+1</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B11" si="0">B3+1</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>